<commit_message>
feature/Excel_Challenge_803 - Max & Min
</commit_message>
<xml_diff>
--- a/Excel_Challenge_801 - Name and Seq.xlsx
+++ b/Excel_Challenge_801 - Name and Seq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VIJAYVERMA\0. Vijay\Excel_Social\Staging\Current Week\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztofnowak/Desktop/ExcelBi/Excel_BI_Challanges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C96CAC7-4A8A-4FE9-95D1-AD831841601C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4B82A0-FF6C-AF46-96C5-58A11F1E00E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -115,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +130,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC8C8C8"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -164,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -173,6 +179,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -635,30 +643,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -674,8 +683,17 @@
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -691,8 +709,29 @@
       <c r="F3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="b">
+        <f>F3=H3</f>
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <f>E3=I3</f>
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <f>D3=J3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -708,8 +747,29 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="shared" ref="K4:K20" si="0">F4=H4</f>
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <f t="shared" ref="L4:L20" si="1">E4=I4</f>
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <f t="shared" ref="M4:M20" si="2">D4=J4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -725,8 +785,29 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -742,8 +823,29 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="5">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -759,8 +861,29 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="5">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>7</v>
       </c>
@@ -770,8 +893,29 @@
       <c r="F8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="5">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>7</v>
       </c>
@@ -781,8 +925,29 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -795,8 +960,29 @@
       <c r="F10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="5">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>20</v>
       </c>
@@ -806,8 +992,29 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="5">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -817,8 +1024,29 @@
       <c r="F12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="5">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M12" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>21</v>
       </c>
@@ -828,8 +1056,29 @@
       <c r="F13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="5">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M13" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>10</v>
       </c>
@@ -839,8 +1088,29 @@
       <c r="F14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="5">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L14" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>20</v>
       </c>
@@ -850,8 +1120,29 @@
       <c r="F15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="5">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>10</v>
       </c>
@@ -861,8 +1152,29 @@
       <c r="F16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="4:6">
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="5">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>20</v>
       </c>
@@ -872,8 +1184,29 @@
       <c r="F17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="4:6">
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="5">
+        <v>15</v>
+      </c>
+      <c r="J17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M17" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>20</v>
       </c>
@@ -883,8 +1216,29 @@
       <c r="F18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="4:6">
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="5">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>10</v>
       </c>
@@ -894,8 +1248,29 @@
       <c r="F19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="4:6">
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="5">
+        <v>17</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>22</v>
       </c>
@@ -905,6 +1280,30 @@
       <c r="F20" t="s">
         <v>8</v>
       </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="5">
+        <v>18</v>
+      </c>
+      <c r="J20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="I21" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A7">
@@ -923,9 +1322,9 @@
       <selection activeCell="G2" sqref="G2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -947,7 +1346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -961,7 +1360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -975,7 +1374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -989,7 +1388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>22</v>
       </c>

</xml_diff>